<commit_message>
Tilpasning til deling og oppdatering av halvårstall
</commit_message>
<xml_diff>
--- a/nedlastede data/buss/2023 Punktlighet versjon3.xlsx
+++ b/nedlastede data/buss/2023 Punktlighet versjon3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtfk.sharepoint.com/sites/SMM-MarkedogUtvikling/Delte dokumenter/Marked, Teknologi og Utvikling/Statistikk/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjo0401\Vestfold og Telemark fylkeskommune\SMM-Marked og Utvikling - Marked, Teknologi og Utvikling\Statistikk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="14_{9DFF6690-8E7C-400C-8C64-015180E5ACDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36031263-CC89-487F-83FB-87EF905C4A62}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D699EBA-B996-4B9F-8B06-6E0441740A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="0" windowWidth="25785" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29880" yWindow="3570" windowWidth="28650" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="1" r:id="rId1"/>
@@ -1307,25 +1307,25 @@
                   <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57000000000000006</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.56999999999999995</c:v>
+                  <c:v>0.59</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.63</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.61</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.72</c:v>
+                  <c:v>0.73</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.41000000000000003</c:v>
+                  <c:v>0.42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1470,25 +1470,25 @@
                   <c:v>0.32999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42999999999999994</c:v>
+                  <c:v>0.43999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.44999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.43000000000000005</c:v>
+                  <c:v>0.41000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.37</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>0.27</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.59</c:v>
+                  <c:v>0.58000000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2226,31 +2226,31 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.59</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2380,31 +2380,31 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.31999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.45999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.31999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0.41000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0.58000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0.20999999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2770,10 +2770,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3122,31 +3122,31 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.56999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.63</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.80500000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3276,31 +3276,31 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.32999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.43000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.36</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.31999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0.37</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.38</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0.19499999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3661,10 +3661,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.80500000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6477,7 +6477,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.60250000000000004</c:v>
+                  <c:v>0.60500000000000009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6765,7 +6765,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.80249999999999999</c:v>
+                  <c:v>0.80083333333333329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -34430,8 +34430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34538,8 +34538,12 @@
       <c r="E7" s="20">
         <v>0.66</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
+      <c r="F7" s="20">
+        <v>0.68</v>
+      </c>
+      <c r="G7" s="20">
+        <v>0.67</v>
+      </c>
       <c r="H7" s="20"/>
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
@@ -34574,8 +34578,12 @@
       <c r="E8" s="20">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
+      <c r="F8" s="20">
+        <v>0.54</v>
+      </c>
+      <c r="G8" s="20">
+        <v>0.56999999999999995</v>
+      </c>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
@@ -34584,11 +34592,11 @@
       <c r="M8" s="20"/>
       <c r="N8" s="20">
         <f>ROUNDUP((AVERAGE(B8:K8)),2)</f>
-        <v>0.57000000000000006</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="O8" s="21">
         <f t="shared" ref="O8:O14" si="0">1-N8</f>
-        <v>0.42999999999999994</v>
+        <v>0.43999999999999995</v>
       </c>
       <c r="P8" s="8"/>
       <c r="Q8" s="10"/>
@@ -34609,8 +34617,12 @@
       <c r="E9" s="20">
         <v>0.54</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
+      <c r="F9" s="20">
+        <v>0.53</v>
+      </c>
+      <c r="G9" s="20">
+        <v>0.53</v>
+      </c>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
@@ -34644,8 +34656,12 @@
       <c r="E10" s="20">
         <v>0.57999999999999996</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
+      <c r="F10" s="20">
+        <v>0.6</v>
+      </c>
+      <c r="G10" s="20">
+        <v>0.64</v>
+      </c>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
@@ -34654,11 +34670,11 @@
       <c r="M10" s="20"/>
       <c r="N10" s="20">
         <f t="shared" si="1"/>
-        <v>0.56999999999999995</v>
+        <v>0.59</v>
       </c>
       <c r="O10" s="21">
         <f t="shared" si="0"/>
-        <v>0.43000000000000005</v>
+        <v>0.41000000000000003</v>
       </c>
       <c r="P10" s="8"/>
       <c r="Q10" s="10"/>
@@ -34679,8 +34695,12 @@
       <c r="E11" s="20">
         <v>0.65</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
+      <c r="F11" s="20">
+        <v>0.68</v>
+      </c>
+      <c r="G11" s="20">
+        <v>0.68</v>
+      </c>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
@@ -34689,11 +34709,11 @@
       <c r="M11" s="20"/>
       <c r="N11" s="20">
         <f t="shared" si="1"/>
-        <v>0.63</v>
+        <v>0.65</v>
       </c>
       <c r="O11" s="21">
         <f t="shared" si="0"/>
-        <v>0.37</v>
+        <v>0.35</v>
       </c>
       <c r="P11" s="8"/>
       <c r="Q11" s="12"/>
@@ -34714,8 +34734,12 @@
       <c r="E12" s="20">
         <v>0.62</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
+      <c r="F12" s="20">
+        <v>0.59</v>
+      </c>
+      <c r="G12" s="20">
+        <v>0.63</v>
+      </c>
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
@@ -34749,8 +34773,12 @@
       <c r="E13" s="20">
         <v>0.77</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
+      <c r="F13" s="20">
+        <v>0.73</v>
+      </c>
+      <c r="G13" s="20">
+        <v>0.76</v>
+      </c>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
       <c r="J13" s="20"/>
@@ -34759,11 +34787,11 @@
       <c r="M13" s="20"/>
       <c r="N13" s="20">
         <f t="shared" si="1"/>
-        <v>0.72</v>
+        <v>0.73</v>
       </c>
       <c r="O13" s="21">
         <f t="shared" si="0"/>
-        <v>0.28000000000000003</v>
+        <v>0.27</v>
       </c>
       <c r="P13" s="8"/>
       <c r="Q13" s="10"/>
@@ -34784,8 +34812,12 @@
       <c r="E14" s="20">
         <v>0.39</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
+      <c r="F14" s="20">
+        <v>0.42</v>
+      </c>
+      <c r="G14" s="20">
+        <v>0.48</v>
+      </c>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
@@ -34794,11 +34826,11 @@
       <c r="M14" s="20"/>
       <c r="N14" s="20">
         <f t="shared" si="1"/>
-        <v>0.41000000000000003</v>
+        <v>0.42</v>
       </c>
       <c r="O14" s="21">
         <f t="shared" si="0"/>
-        <v>0.59</v>
+        <v>0.58000000000000007</v>
       </c>
       <c r="P14" s="8"/>
       <c r="Q14" s="12"/>
@@ -34838,8 +34870,12 @@
       <c r="E16" s="82">
         <v>0.6</v>
       </c>
-      <c r="F16" s="80"/>
-      <c r="G16" s="80"/>
+      <c r="F16" s="82">
+        <v>0.6</v>
+      </c>
+      <c r="G16" s="80">
+        <v>0.62</v>
+      </c>
       <c r="H16" s="80"/>
       <c r="I16" s="80"/>
       <c r="J16" s="80"/>
@@ -34848,11 +34884,11 @@
       <c r="M16" s="80"/>
       <c r="N16" s="79">
         <f>AVERAGE(B16:M16)</f>
-        <v>0.60250000000000004</v>
+        <v>0.60500000000000009</v>
       </c>
       <c r="O16" s="79">
         <f>1-N16</f>
-        <v>0.39749999999999996</v>
+        <v>0.39499999999999991</v>
       </c>
       <c r="P16" s="69"/>
       <c r="Q16" s="16"/>
@@ -34873,8 +34909,12 @@
       <c r="E17" s="80">
         <v>0.79</v>
       </c>
-      <c r="F17" s="80"/>
-      <c r="G17" s="80"/>
+      <c r="F17" s="80">
+        <v>0.79</v>
+      </c>
+      <c r="G17" s="80">
+        <v>0.80500000000000005</v>
+      </c>
       <c r="H17" s="80"/>
       <c r="I17" s="80"/>
       <c r="J17" s="80"/>
@@ -34883,11 +34923,11 @@
       <c r="M17" s="80"/>
       <c r="N17" s="79">
         <f>AVERAGE(B17:M17)</f>
-        <v>0.80249999999999999</v>
+        <v>0.80083333333333329</v>
       </c>
       <c r="O17" s="79">
         <f>1-N17</f>
-        <v>0.19750000000000001</v>
+        <v>0.19916666666666671</v>
       </c>
       <c r="P17" s="70"/>
       <c r="Q17" s="18"/>
@@ -34989,14 +35029,14 @@
       </c>
       <c r="B47" s="22">
         <f>F16</f>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="C47" s="22">
         <v>0.6</v>
       </c>
       <c r="D47" s="22">
         <f>F17</f>
-        <v>0</v>
+        <v>0.79</v>
       </c>
       <c r="E47" s="24">
         <v>0.93</v>
@@ -35008,14 +35048,14 @@
       </c>
       <c r="B48" s="22">
         <f>G16</f>
-        <v>0</v>
+        <v>0.62</v>
       </c>
       <c r="C48" s="22">
         <v>0.61</v>
       </c>
       <c r="D48" s="22">
         <f>G17</f>
-        <v>0</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="E48" s="24">
         <v>0.8</v>
@@ -35141,14 +35181,14 @@
       </c>
       <c r="B55" s="26">
         <f>N16</f>
-        <v>0.60250000000000004</v>
+        <v>0.60500000000000009</v>
       </c>
       <c r="C55" s="26">
         <v>0.64416666666666667</v>
       </c>
       <c r="D55" s="26">
         <f>N17</f>
-        <v>0.80249999999999999</v>
+        <v>0.80083333333333329</v>
       </c>
       <c r="E55" s="27">
         <v>0.85583333333333345</v>
@@ -36530,11 +36570,11 @@
       </c>
       <c r="B1" s="62">
         <f>Total!F7</f>
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="C1" s="32">
         <f>D1-B1</f>
-        <v>1</v>
+        <v>0.31999999999999995</v>
       </c>
       <c r="D1" s="33">
         <v>1</v>
@@ -36546,11 +36586,11 @@
       </c>
       <c r="B2" s="20">
         <f>Total!F8</f>
-        <v>0</v>
+        <v>0.54</v>
       </c>
       <c r="C2" s="21">
         <f t="shared" ref="C2:C10" si="0">D2-B2</f>
-        <v>1</v>
+        <v>0.45999999999999996</v>
       </c>
       <c r="D2" s="35">
         <v>1</v>
@@ -36562,11 +36602,11 @@
       </c>
       <c r="B3" s="20">
         <f>Total!F9</f>
-        <v>0</v>
+        <v>0.53</v>
       </c>
       <c r="C3" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.47</v>
       </c>
       <c r="D3" s="35">
         <v>1</v>
@@ -36578,11 +36618,11 @@
       </c>
       <c r="B4" s="20">
         <f>Total!F10</f>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="C4" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D4" s="35">
         <v>1</v>
@@ -36594,11 +36634,11 @@
       </c>
       <c r="B5" s="20">
         <f>Total!F11</f>
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="C5" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.31999999999999995</v>
       </c>
       <c r="D5" s="35">
         <v>1</v>
@@ -36610,11 +36650,11 @@
       </c>
       <c r="B6" s="20">
         <f>Total!F12</f>
-        <v>0</v>
+        <v>0.59</v>
       </c>
       <c r="C6" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.41000000000000003</v>
       </c>
       <c r="D6" s="35">
         <v>1</v>
@@ -36626,11 +36666,11 @@
       </c>
       <c r="B7" s="66">
         <f>Total!F14</f>
-        <v>0</v>
+        <v>0.42</v>
       </c>
       <c r="C7" s="37">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.58000000000000007</v>
       </c>
       <c r="D7" s="38">
         <v>1</v>
@@ -36648,11 +36688,11 @@
       </c>
       <c r="B9" s="19">
         <f>Total!B47</f>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="C9" s="52">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D9" s="53">
         <v>1</v>
@@ -36664,11 +36704,11 @@
       </c>
       <c r="B10" s="51">
         <f>Total!D47</f>
-        <v>0</v>
+        <v>0.79</v>
       </c>
       <c r="C10" s="52">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.20999999999999996</v>
       </c>
       <c r="D10" s="53">
         <v>1</v>
@@ -36699,11 +36739,11 @@
       </c>
       <c r="B1" s="62">
         <f>Total!G7</f>
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="C1" s="32">
         <f>D1-B1</f>
-        <v>1</v>
+        <v>0.32999999999999996</v>
       </c>
       <c r="D1" s="33">
         <v>1</v>
@@ -36715,11 +36755,11 @@
       </c>
       <c r="B2" s="20">
         <f>Total!G8</f>
-        <v>0</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="C2" s="21">
         <f t="shared" ref="C2:C10" si="0">D2-B2</f>
-        <v>1</v>
+        <v>0.43000000000000005</v>
       </c>
       <c r="D2" s="35">
         <v>1</v>
@@ -36731,11 +36771,11 @@
       </c>
       <c r="B3" s="20">
         <f>Total!G9</f>
-        <v>0</v>
+        <v>0.53</v>
       </c>
       <c r="C3" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.47</v>
       </c>
       <c r="D3" s="35">
         <v>1</v>
@@ -36747,11 +36787,11 @@
       </c>
       <c r="B4" s="20">
         <f>Total!G10</f>
-        <v>0</v>
+        <v>0.64</v>
       </c>
       <c r="C4" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.36</v>
       </c>
       <c r="D4" s="35">
         <v>1</v>
@@ -36763,11 +36803,11 @@
       </c>
       <c r="B5" s="20">
         <f>Total!G11</f>
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="C5" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.31999999999999995</v>
       </c>
       <c r="D5" s="35">
         <v>1</v>
@@ -36779,11 +36819,11 @@
       </c>
       <c r="B6" s="20">
         <f>Total!G12</f>
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="C6" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.37</v>
       </c>
       <c r="D6" s="35">
         <v>1</v>
@@ -36795,11 +36835,11 @@
       </c>
       <c r="B7" s="66">
         <f>Total!G14</f>
-        <v>0</v>
+        <v>0.48</v>
       </c>
       <c r="C7" s="37">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.52</v>
       </c>
       <c r="D7" s="38">
         <v>1</v>
@@ -36817,11 +36857,11 @@
       </c>
       <c r="B9" s="19">
         <f>Total!B48</f>
-        <v>0</v>
+        <v>0.62</v>
       </c>
       <c r="C9" s="52">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.38</v>
       </c>
       <c r="D9" s="53">
         <v>1</v>
@@ -36833,11 +36873,11 @@
       </c>
       <c r="B10" s="51">
         <f>Total!D48</f>
-        <v>0</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="C10" s="52">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.19499999999999995</v>
       </c>
       <c r="D10" s="53">
         <v>1</v>

</xml_diff>

<commit_message>
oppdatering med juli 2023
</commit_message>
<xml_diff>
--- a/nedlastede data/buss/2023 Punktlighet versjon3.xlsx
+++ b/nedlastede data/buss/2023 Punktlighet versjon3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjo0401\Vestfold og Telemark fylkeskommune\SMM-Marked og Utvikling - Marked, Teknologi og Utvikling\Statistikk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtfk.sharepoint.com/sites/SMM-MarkedogUtvikling/Delte dokumenter/Marked, Teknologi og Utvikling/Statistikk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D699EBA-B996-4B9F-8B06-6E0441740A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{F52172D5-E799-4600-8311-E961BE524F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29880" yWindow="3570" windowWidth="28650" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29865" yWindow="360" windowWidth="30120" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="1" r:id="rId1"/>
@@ -1304,28 +1304,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>0.69000000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57000000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.67</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.56000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.55000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.59</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.65</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.61</c:v>
+                  <c:v>0.63</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.73</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.42</c:v>
+                  <c:v>0.47000000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1467,28 +1467,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>0.30999999999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42999999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.32999999999999996</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.43999999999999995</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.44999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.41000000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.35</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.39</c:v>
+                  <c:v>0.37</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.27</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.58000000000000007</c:v>
+                  <c:v>0.53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4013,31 +4013,31 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.73</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.73</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4167,31 +4167,31 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.22999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0.27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.21999999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.20999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0.27</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.22999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>6.9999999999999951E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4572,10 +4572,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6477,7 +6477,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.60500000000000009</c:v>
+                  <c:v>0.62857142857142867</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6765,7 +6765,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.80083333333333329</c:v>
+                  <c:v>0.81928571428571417</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -34431,7 +34431,7 @@
   <dimension ref="A2:S55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34544,7 +34544,9 @@
       <c r="G7" s="20">
         <v>0.67</v>
       </c>
-      <c r="H7" s="20"/>
+      <c r="H7" s="20">
+        <v>0.77</v>
+      </c>
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
@@ -34552,11 +34554,11 @@
       <c r="M7" s="20"/>
       <c r="N7" s="20">
         <f>ROUNDUP((AVERAGE(B7:K7)),2)</f>
-        <v>0.67</v>
+        <v>0.69000000000000006</v>
       </c>
       <c r="O7" s="21">
         <f>1-N7</f>
-        <v>0.32999999999999996</v>
+        <v>0.30999999999999994</v>
       </c>
       <c r="P7" s="8"/>
       <c r="Q7" s="9"/>
@@ -34584,7 +34586,9 @@
       <c r="G8" s="20">
         <v>0.56999999999999995</v>
       </c>
-      <c r="H8" s="20"/>
+      <c r="H8" s="20">
+        <v>0.76</v>
+      </c>
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
@@ -34592,11 +34596,11 @@
       <c r="M8" s="20"/>
       <c r="N8" s="20">
         <f>ROUNDUP((AVERAGE(B8:K8)),2)</f>
-        <v>0.56000000000000005</v>
+        <v>0.59</v>
       </c>
       <c r="O8" s="21">
         <f t="shared" ref="O8:O14" si="0">1-N8</f>
-        <v>0.43999999999999995</v>
+        <v>0.41000000000000003</v>
       </c>
       <c r="P8" s="8"/>
       <c r="Q8" s="10"/>
@@ -34623,7 +34627,9 @@
       <c r="G9" s="20">
         <v>0.53</v>
       </c>
-      <c r="H9" s="20"/>
+      <c r="H9" s="20">
+        <v>0.73</v>
+      </c>
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
@@ -34631,11 +34637,11 @@
       <c r="M9" s="20"/>
       <c r="N9" s="20">
         <f t="shared" ref="N9:N14" si="1">ROUNDUP((AVERAGE(B9:K9)),2)</f>
-        <v>0.55000000000000004</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="O9" s="21">
         <f t="shared" si="0"/>
-        <v>0.44999999999999996</v>
+        <v>0.42999999999999994</v>
       </c>
       <c r="P9" s="8"/>
       <c r="Q9" s="9"/>
@@ -34662,7 +34668,9 @@
       <c r="G10" s="20">
         <v>0.64</v>
       </c>
-      <c r="H10" s="20"/>
+      <c r="H10" s="20">
+        <v>0.78</v>
+      </c>
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
@@ -34670,11 +34678,11 @@
       <c r="M10" s="20"/>
       <c r="N10" s="20">
         <f t="shared" si="1"/>
-        <v>0.59</v>
+        <v>0.62</v>
       </c>
       <c r="O10" s="21">
         <f t="shared" si="0"/>
-        <v>0.41000000000000003</v>
+        <v>0.38</v>
       </c>
       <c r="P10" s="8"/>
       <c r="Q10" s="10"/>
@@ -34701,7 +34709,9 @@
       <c r="G11" s="20">
         <v>0.68</v>
       </c>
-      <c r="H11" s="20"/>
+      <c r="H11" s="20">
+        <v>0.79</v>
+      </c>
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
@@ -34709,11 +34719,11 @@
       <c r="M11" s="20"/>
       <c r="N11" s="20">
         <f t="shared" si="1"/>
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
       <c r="O11" s="21">
         <f t="shared" si="0"/>
-        <v>0.35</v>
+        <v>0.32999999999999996</v>
       </c>
       <c r="P11" s="8"/>
       <c r="Q11" s="12"/>
@@ -34740,7 +34750,9 @@
       <c r="G12" s="20">
         <v>0.63</v>
       </c>
-      <c r="H12" s="20"/>
+      <c r="H12" s="20">
+        <v>0.75</v>
+      </c>
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
@@ -34748,11 +34760,11 @@
       <c r="M12" s="20"/>
       <c r="N12" s="20">
         <f t="shared" si="1"/>
-        <v>0.61</v>
+        <v>0.63</v>
       </c>
       <c r="O12" s="21">
         <f t="shared" si="0"/>
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="P12" s="8"/>
       <c r="Q12" s="10"/>
@@ -34779,7 +34791,9 @@
       <c r="G13" s="20">
         <v>0.76</v>
       </c>
-      <c r="H13" s="20"/>
+      <c r="H13" s="20">
+        <v>0.9</v>
+      </c>
       <c r="I13" s="20"/>
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
@@ -34787,11 +34801,11 @@
       <c r="M13" s="20"/>
       <c r="N13" s="20">
         <f t="shared" si="1"/>
-        <v>0.73</v>
+        <v>0.75</v>
       </c>
       <c r="O13" s="21">
         <f t="shared" si="0"/>
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="P13" s="8"/>
       <c r="Q13" s="10"/>
@@ -34818,7 +34832,9 @@
       <c r="G14" s="20">
         <v>0.48</v>
       </c>
-      <c r="H14" s="20"/>
+      <c r="H14" s="20">
+        <v>0.73</v>
+      </c>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
@@ -34826,11 +34842,11 @@
       <c r="M14" s="20"/>
       <c r="N14" s="20">
         <f t="shared" si="1"/>
-        <v>0.42</v>
+        <v>0.47000000000000003</v>
       </c>
       <c r="O14" s="21">
         <f t="shared" si="0"/>
-        <v>0.58000000000000007</v>
+        <v>0.53</v>
       </c>
       <c r="P14" s="8"/>
       <c r="Q14" s="12"/>
@@ -34876,7 +34892,9 @@
       <c r="G16" s="80">
         <v>0.62</v>
       </c>
-      <c r="H16" s="80"/>
+      <c r="H16" s="80">
+        <v>0.77</v>
+      </c>
       <c r="I16" s="80"/>
       <c r="J16" s="80"/>
       <c r="K16" s="80"/>
@@ -34884,11 +34902,11 @@
       <c r="M16" s="80"/>
       <c r="N16" s="79">
         <f>AVERAGE(B16:M16)</f>
-        <v>0.60500000000000009</v>
+        <v>0.62857142857142867</v>
       </c>
       <c r="O16" s="79">
         <f>1-N16</f>
-        <v>0.39499999999999991</v>
+        <v>0.37142857142857133</v>
       </c>
       <c r="P16" s="69"/>
       <c r="Q16" s="16"/>
@@ -34915,7 +34933,9 @@
       <c r="G17" s="80">
         <v>0.80500000000000005</v>
       </c>
-      <c r="H17" s="80"/>
+      <c r="H17" s="80">
+        <v>0.93</v>
+      </c>
       <c r="I17" s="80"/>
       <c r="J17" s="80"/>
       <c r="K17" s="80"/>
@@ -34923,11 +34943,11 @@
       <c r="M17" s="80"/>
       <c r="N17" s="79">
         <f>AVERAGE(B17:M17)</f>
-        <v>0.80083333333333329</v>
+        <v>0.81928571428571417</v>
       </c>
       <c r="O17" s="79">
         <f>1-N17</f>
-        <v>0.19916666666666671</v>
+        <v>0.18071428571428583</v>
       </c>
       <c r="P17" s="70"/>
       <c r="Q17" s="18"/>
@@ -35067,14 +35087,14 @@
       </c>
       <c r="B49" s="22">
         <f>H16</f>
-        <v>0</v>
+        <v>0.77</v>
       </c>
       <c r="C49" s="22">
         <v>0.78</v>
       </c>
       <c r="D49" s="22">
         <f>H17</f>
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="E49" s="24">
         <v>0.9</v>
@@ -35181,14 +35201,14 @@
       </c>
       <c r="B55" s="26">
         <f>N16</f>
-        <v>0.60500000000000009</v>
+        <v>0.62857142857142867</v>
       </c>
       <c r="C55" s="26">
         <v>0.64416666666666667</v>
       </c>
       <c r="D55" s="26">
         <f>N17</f>
-        <v>0.80083333333333329</v>
+        <v>0.81928571428571417</v>
       </c>
       <c r="E55" s="27">
         <v>0.85583333333333345</v>
@@ -36908,11 +36928,11 @@
       </c>
       <c r="B1" s="62">
         <f>Total!H7</f>
-        <v>0</v>
+        <v>0.77</v>
       </c>
       <c r="C1" s="32">
         <f>D1-B1</f>
-        <v>1</v>
+        <v>0.22999999999999998</v>
       </c>
       <c r="D1" s="33">
         <v>1</v>
@@ -36924,11 +36944,11 @@
       </c>
       <c r="B2" s="20">
         <f>Total!H8</f>
-        <v>0</v>
+        <v>0.76</v>
       </c>
       <c r="C2" s="21">
         <f t="shared" ref="C2:C10" si="0">D2-B2</f>
-        <v>1</v>
+        <v>0.24</v>
       </c>
       <c r="D2" s="35">
         <v>1</v>
@@ -36940,11 +36960,11 @@
       </c>
       <c r="B3" s="20">
         <f>Total!H9</f>
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="C3" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.27</v>
       </c>
       <c r="D3" s="35">
         <v>1</v>
@@ -36956,11 +36976,11 @@
       </c>
       <c r="B4" s="20">
         <f>Total!H10</f>
-        <v>0</v>
+        <v>0.78</v>
       </c>
       <c r="C4" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.21999999999999997</v>
       </c>
       <c r="D4" s="35">
         <v>1</v>
@@ -36972,11 +36992,11 @@
       </c>
       <c r="B5" s="20">
         <f>Total!H11</f>
-        <v>0</v>
+        <v>0.79</v>
       </c>
       <c r="C5" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.20999999999999996</v>
       </c>
       <c r="D5" s="35">
         <v>1</v>
@@ -36988,11 +37008,11 @@
       </c>
       <c r="B6" s="20">
         <f>Total!H12</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="C6" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D6" s="35">
         <v>1</v>
@@ -37004,11 +37024,11 @@
       </c>
       <c r="B7" s="66">
         <f>Total!H14</f>
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="C7" s="37">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.27</v>
       </c>
       <c r="D7" s="38">
         <v>1</v>
@@ -37026,11 +37046,11 @@
       </c>
       <c r="B9" s="19">
         <f>Total!B49</f>
-        <v>0</v>
+        <v>0.77</v>
       </c>
       <c r="C9" s="52">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.22999999999999998</v>
       </c>
       <c r="D9" s="53">
         <v>1</v>
@@ -37042,11 +37062,11 @@
       </c>
       <c r="B10" s="51">
         <f>Total!D49</f>
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="C10" s="52">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>6.9999999999999951E-2</v>
       </c>
       <c r="D10" s="53">
         <v>1</v>
@@ -37228,19 +37248,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="478e6b58-aec7-4dc3-9f41-cb49fd51aa76" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de218069-9b18-4834-8a42-87538bc414b8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001898DE31E6781040974FAF2B6226B070" ma:contentTypeVersion="16" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="a7c44ff76577bc4f25f19cca4255138f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="de218069-9b18-4834-8a42-87538bc414b8" xmlns:ns3="346015c6-8778-4c47-bc51-98fcc3d8f0cc" xmlns:ns4="478e6b58-aec7-4dc3-9f41-cb49fd51aa76" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ca1f1bffadeb320ffeb9037f02edf329" ns2:_="" ns3:_="" ns4:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001898DE31E6781040974FAF2B6226B070" ma:contentTypeVersion="17" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="8210ab889ee5475f8279815924805e7a">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="de218069-9b18-4834-8a42-87538bc414b8" xmlns:ns3="346015c6-8778-4c47-bc51-98fcc3d8f0cc" xmlns:ns4="478e6b58-aec7-4dc3-9f41-cb49fd51aa76" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2ca27dc987c1ae5dda2f1ddae95e9c5a" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="de218069-9b18-4834-8a42-87538bc414b8"/>
     <xsd:import namespace="346015c6-8778-4c47-bc51-98fcc3d8f0cc"/>
     <xsd:import namespace="478e6b58-aec7-4dc3-9f41-cb49fd51aa76"/>
@@ -37265,6 +37274,7 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns4:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -37340,6 +37350,11 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="346015c6-8778-4c47-bc51-98fcc3d8f0cc" elementFormDefault="qualified">
@@ -37486,6 +37501,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="478e6b58-aec7-4dc3-9f41-cb49fd51aa76" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de218069-9b18-4834-8a42-87538bc414b8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -37496,6 +37522,10 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4888F49C-1AE0-4EBF-A654-04D8E1B2E686}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E51255DE-438C-4222-9FEF-BAA467D81EC9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -37503,26 +37533,6 @@
     <ds:schemaRef ds:uri="1be84928-a867-465e-b2ee-3fc273237fa1"/>
     <ds:schemaRef ds:uri="478e6b58-aec7-4dc3-9f41-cb49fd51aa76"/>
     <ds:schemaRef ds:uri="de218069-9b18-4834-8a42-87538bc414b8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A37010C-966A-4084-B0FD-C98F93645BE9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="de218069-9b18-4834-8a42-87538bc414b8"/>
-    <ds:schemaRef ds:uri="346015c6-8778-4c47-bc51-98fcc3d8f0cc"/>
-    <ds:schemaRef ds:uri="478e6b58-aec7-4dc3-9f41-cb49fd51aa76"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Passasjertall tom august 2023
</commit_message>
<xml_diff>
--- a/nedlastede data/buss/2023 Punktlighet versjon3.xlsx
+++ b/nedlastede data/buss/2023 Punktlighet versjon3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtfk.sharepoint.com/sites/SMM-MarkedogUtvikling/Delte dokumenter/Marked, Teknologi og Utvikling/Statistikk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{F52172D5-E799-4600-8311-E961BE524F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{AF410301-6D27-4E4E-A11C-5AF53E1ADD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29865" yWindow="360" windowWidth="30120" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36120" yWindow="1530" windowWidth="21570" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="1" r:id="rId1"/>
@@ -1316,10 +1316,10 @@
                   <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.67</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.63</c:v>
+                  <c:v>0.64</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.75</c:v>
@@ -1479,10 +1479,10 @@
                   <c:v>0.38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32999999999999996</c:v>
+                  <c:v>0.31999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.37</c:v>
+                  <c:v>0.36</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.25</c:v>
@@ -4929,31 +4929,31 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.56999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.61</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.63</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5083,31 +5083,31 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.32999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.43000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0.43999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0.33999999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.37</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0.19999999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5497,10 +5497,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6477,7 +6477,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.62857142857142867</c:v>
+                  <c:v>0.62875000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6765,7 +6765,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.81928571428571417</c:v>
+                  <c:v>0.81687499999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -34431,7 +34431,7 @@
   <dimension ref="A2:S55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34547,7 +34547,9 @@
       <c r="H7" s="20">
         <v>0.77</v>
       </c>
-      <c r="I7" s="20"/>
+      <c r="I7" s="20">
+        <v>0.67</v>
+      </c>
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
       <c r="L7" s="20"/>
@@ -34589,7 +34591,9 @@
       <c r="H8" s="20">
         <v>0.76</v>
       </c>
-      <c r="I8" s="20"/>
+      <c r="I8" s="20">
+        <v>0.56999999999999995</v>
+      </c>
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
@@ -34630,7 +34634,9 @@
       <c r="H9" s="20">
         <v>0.73</v>
       </c>
-      <c r="I9" s="20"/>
+      <c r="I9" s="20">
+        <v>0.56000000000000005</v>
+      </c>
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
@@ -34671,7 +34677,9 @@
       <c r="H10" s="20">
         <v>0.78</v>
       </c>
-      <c r="I10" s="20"/>
+      <c r="I10" s="20">
+        <v>0.61</v>
+      </c>
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
@@ -34712,18 +34720,20 @@
       <c r="H11" s="20">
         <v>0.79</v>
       </c>
-      <c r="I11" s="20"/>
+      <c r="I11" s="20">
+        <v>0.7</v>
+      </c>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
       <c r="N11" s="20">
         <f t="shared" si="1"/>
-        <v>0.67</v>
+        <v>0.68</v>
       </c>
       <c r="O11" s="21">
         <f t="shared" si="0"/>
-        <v>0.32999999999999996</v>
+        <v>0.31999999999999995</v>
       </c>
       <c r="P11" s="8"/>
       <c r="Q11" s="12"/>
@@ -34753,18 +34763,20 @@
       <c r="H12" s="20">
         <v>0.75</v>
       </c>
-      <c r="I12" s="20"/>
+      <c r="I12" s="20">
+        <v>0.66</v>
+      </c>
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
       <c r="N12" s="20">
         <f t="shared" si="1"/>
-        <v>0.63</v>
+        <v>0.64</v>
       </c>
       <c r="O12" s="21">
         <f t="shared" si="0"/>
-        <v>0.37</v>
+        <v>0.36</v>
       </c>
       <c r="P12" s="8"/>
       <c r="Q12" s="10"/>
@@ -34794,7 +34806,9 @@
       <c r="H13" s="20">
         <v>0.9</v>
       </c>
-      <c r="I13" s="20"/>
+      <c r="I13" s="20">
+        <v>0.73</v>
+      </c>
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
@@ -34835,7 +34849,9 @@
       <c r="H14" s="20">
         <v>0.73</v>
       </c>
-      <c r="I14" s="20"/>
+      <c r="I14" s="20">
+        <v>0.5</v>
+      </c>
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
@@ -34895,18 +34911,20 @@
       <c r="H16" s="80">
         <v>0.77</v>
       </c>
-      <c r="I16" s="80"/>
+      <c r="I16" s="80">
+        <v>0.63</v>
+      </c>
       <c r="J16" s="80"/>
       <c r="K16" s="80"/>
       <c r="L16" s="80"/>
       <c r="M16" s="80"/>
       <c r="N16" s="79">
         <f>AVERAGE(B16:M16)</f>
-        <v>0.62857142857142867</v>
+        <v>0.62875000000000003</v>
       </c>
       <c r="O16" s="79">
         <f>1-N16</f>
-        <v>0.37142857142857133</v>
+        <v>0.37124999999999997</v>
       </c>
       <c r="P16" s="69"/>
       <c r="Q16" s="16"/>
@@ -34936,18 +34954,20 @@
       <c r="H17" s="80">
         <v>0.93</v>
       </c>
-      <c r="I17" s="80"/>
+      <c r="I17" s="80">
+        <v>0.8</v>
+      </c>
       <c r="J17" s="80"/>
       <c r="K17" s="80"/>
       <c r="L17" s="80"/>
       <c r="M17" s="80"/>
       <c r="N17" s="79">
         <f>AVERAGE(B17:M17)</f>
-        <v>0.81928571428571417</v>
+        <v>0.81687499999999991</v>
       </c>
       <c r="O17" s="79">
         <f>1-N17</f>
-        <v>0.18071428571428583</v>
+        <v>0.18312500000000009</v>
       </c>
       <c r="P17" s="70"/>
       <c r="Q17" s="18"/>
@@ -35106,14 +35126,14 @@
       </c>
       <c r="B50" s="22">
         <f>I16</f>
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="C50" s="22">
         <v>0.65</v>
       </c>
       <c r="D50" s="22">
         <f>I17</f>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E50" s="24">
         <v>0.79</v>
@@ -35201,14 +35221,14 @@
       </c>
       <c r="B55" s="26">
         <f>N16</f>
-        <v>0.62857142857142867</v>
+        <v>0.62875000000000003</v>
       </c>
       <c r="C55" s="26">
         <v>0.64416666666666667</v>
       </c>
       <c r="D55" s="26">
         <f>N17</f>
-        <v>0.81928571428571417</v>
+        <v>0.81687499999999991</v>
       </c>
       <c r="E55" s="27">
         <v>0.85583333333333345</v>
@@ -37097,11 +37117,11 @@
       </c>
       <c r="B1" s="62">
         <f>Total!I7</f>
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="C1" s="32">
         <f>D1-B1</f>
-        <v>1</v>
+        <v>0.32999999999999996</v>
       </c>
       <c r="D1" s="33">
         <v>1</v>
@@ -37113,11 +37133,11 @@
       </c>
       <c r="B2" s="20">
         <f>Total!I8</f>
-        <v>0</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="C2" s="21">
         <f t="shared" ref="C2:C10" si="0">D2-B2</f>
-        <v>1</v>
+        <v>0.43000000000000005</v>
       </c>
       <c r="D2" s="35">
         <v>1</v>
@@ -37129,11 +37149,11 @@
       </c>
       <c r="B3" s="20">
         <f>Total!I9</f>
-        <v>0</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="C3" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.43999999999999995</v>
       </c>
       <c r="D3" s="35">
         <v>1</v>
@@ -37145,11 +37165,11 @@
       </c>
       <c r="B4" s="20">
         <f>Total!I10</f>
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="C4" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.39</v>
       </c>
       <c r="D4" s="35">
         <v>1</v>
@@ -37161,11 +37181,11 @@
       </c>
       <c r="B5" s="20">
         <f>Total!I11</f>
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="C5" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="D5" s="35">
         <v>1</v>
@@ -37177,11 +37197,11 @@
       </c>
       <c r="B6" s="20">
         <f>Total!I12</f>
-        <v>0</v>
+        <v>0.66</v>
       </c>
       <c r="C6" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.33999999999999997</v>
       </c>
       <c r="D6" s="35">
         <v>1</v>
@@ -37193,11 +37213,11 @@
       </c>
       <c r="B7" s="66">
         <f>Total!I14</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C7" s="37">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D7" s="38">
         <v>1</v>
@@ -37215,11 +37235,11 @@
       </c>
       <c r="B9" s="19">
         <f>Total!B50</f>
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="C9" s="52">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.37</v>
       </c>
       <c r="D9" s="53">
         <v>1</v>
@@ -37231,11 +37251,11 @@
       </c>
       <c r="B10" s="51">
         <f>Total!D50</f>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="C10" s="52">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="D10" s="53">
         <v>1</v>
@@ -37248,6 +37268,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="478e6b58-aec7-4dc3-9f41-cb49fd51aa76" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de218069-9b18-4834-8a42-87538bc414b8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001898DE31E6781040974FAF2B6226B070" ma:contentTypeVersion="17" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="8210ab889ee5475f8279815924805e7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="de218069-9b18-4834-8a42-87538bc414b8" xmlns:ns3="346015c6-8778-4c47-bc51-98fcc3d8f0cc" xmlns:ns4="478e6b58-aec7-4dc3-9f41-cb49fd51aa76" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2ca27dc987c1ae5dda2f1ddae95e9c5a" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="de218069-9b18-4834-8a42-87538bc414b8"/>
@@ -37501,17 +37532,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="478e6b58-aec7-4dc3-9f41-cb49fd51aa76" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de218069-9b18-4834-8a42-87538bc414b8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -37522,10 +37542,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4888F49C-1AE0-4EBF-A654-04D8E1B2E686}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E51255DE-438C-4222-9FEF-BAA467D81EC9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -37533,6 +37549,26 @@
     <ds:schemaRef ds:uri="1be84928-a867-465e-b2ee-3fc273237fa1"/>
     <ds:schemaRef ds:uri="478e6b58-aec7-4dc3-9f41-cb49fd51aa76"/>
     <ds:schemaRef ds:uri="de218069-9b18-4834-8a42-87538bc414b8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4888F49C-1AE0-4EBF-A654-04D8E1B2E686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="de218069-9b18-4834-8a42-87538bc414b8"/>
+    <ds:schemaRef ds:uri="346015c6-8778-4c47-bc51-98fcc3d8f0cc"/>
+    <ds:schemaRef ds:uri="478e6b58-aec7-4dc3-9f41-cb49fd51aa76"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update 2023 Punktlighet versjon3.xlsx
</commit_message>
<xml_diff>
--- a/nedlastede data/buss/2023 Punktlighet versjon3.xlsx
+++ b/nedlastede data/buss/2023 Punktlighet versjon3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtfk.sharepoint.com/sites/SMM-MarkedogUtvikling/Delte dokumenter/Marked, Teknologi og Utvikling/Statistikk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{AF410301-6D27-4E4E-A11C-5AF53E1ADD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{228C2F27-4051-4751-97D8-DDE3C72244CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36120" yWindow="1530" windowWidth="21570" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27270" yWindow="630" windowWidth="30270" windowHeight="14835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="1" r:id="rId1"/>
@@ -1304,7 +1304,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.69000000000000006</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.59</c:v>
@@ -1313,10 +1313,10 @@
                   <c:v>0.57000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.62</c:v>
+                  <c:v>0.61</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.68</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.64</c:v>
@@ -1467,7 +1467,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.30999999999999994</c:v>
+                  <c:v>0.31999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.41000000000000003</c:v>
@@ -1476,10 +1476,10 @@
                   <c:v>0.42999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.38</c:v>
+                  <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.31999999999999995</c:v>
+                  <c:v>0.32999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.36</c:v>
@@ -5849,31 +5849,31 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.61</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6003,31 +6003,31 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.32999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.43999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0.43999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.44999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0.18999999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6477,7 +6477,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.62875000000000003</c:v>
+                  <c:v>0.62666666666666671</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6765,7 +6765,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.81687499999999991</c:v>
+                  <c:v>0.81611111111111101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7337,10 +7337,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.61</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -34431,7 +34431,7 @@
   <dimension ref="A2:S55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34550,17 +34550,19 @@
       <c r="I7" s="20">
         <v>0.67</v>
       </c>
-      <c r="J7" s="20"/>
+      <c r="J7" s="20">
+        <v>0.67</v>
+      </c>
       <c r="K7" s="20"/>
       <c r="L7" s="20"/>
       <c r="M7" s="20"/>
       <c r="N7" s="20">
         <f>ROUNDUP((AVERAGE(B7:K7)),2)</f>
-        <v>0.69000000000000006</v>
+        <v>0.68</v>
       </c>
       <c r="O7" s="21">
         <f>1-N7</f>
-        <v>0.30999999999999994</v>
+        <v>0.31999999999999995</v>
       </c>
       <c r="P7" s="8"/>
       <c r="Q7" s="9"/>
@@ -34594,7 +34596,9 @@
       <c r="I8" s="20">
         <v>0.56999999999999995</v>
       </c>
-      <c r="J8" s="20"/>
+      <c r="J8" s="20">
+        <v>0.56000000000000005</v>
+      </c>
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
@@ -34637,7 +34641,9 @@
       <c r="I9" s="20">
         <v>0.56000000000000005</v>
       </c>
-      <c r="J9" s="20"/>
+      <c r="J9" s="20">
+        <v>0.56000000000000005</v>
+      </c>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
@@ -34680,17 +34686,19 @@
       <c r="I10" s="20">
         <v>0.61</v>
       </c>
-      <c r="J10" s="20"/>
+      <c r="J10" s="20">
+        <v>0.55000000000000004</v>
+      </c>
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="20">
         <f t="shared" si="1"/>
-        <v>0.62</v>
+        <v>0.61</v>
       </c>
       <c r="O10" s="21">
         <f t="shared" si="0"/>
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="P10" s="8"/>
       <c r="Q10" s="10"/>
@@ -34723,17 +34731,19 @@
       <c r="I11" s="20">
         <v>0.7</v>
       </c>
-      <c r="J11" s="20"/>
+      <c r="J11" s="20">
+        <v>0.65</v>
+      </c>
       <c r="K11" s="20"/>
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
       <c r="N11" s="20">
         <f t="shared" si="1"/>
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="O11" s="21">
         <f t="shared" si="0"/>
-        <v>0.31999999999999995</v>
+        <v>0.32999999999999996</v>
       </c>
       <c r="P11" s="8"/>
       <c r="Q11" s="12"/>
@@ -34766,7 +34776,9 @@
       <c r="I12" s="20">
         <v>0.66</v>
       </c>
-      <c r="J12" s="20"/>
+      <c r="J12" s="20">
+        <v>0.65</v>
+      </c>
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
@@ -34809,7 +34821,9 @@
       <c r="I13" s="20">
         <v>0.73</v>
       </c>
-      <c r="J13" s="20"/>
+      <c r="J13" s="20">
+        <v>0.76</v>
+      </c>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
@@ -34852,7 +34866,9 @@
       <c r="I14" s="20">
         <v>0.5</v>
       </c>
-      <c r="J14" s="20"/>
+      <c r="J14" s="20">
+        <v>0.45</v>
+      </c>
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
@@ -34914,17 +34930,19 @@
       <c r="I16" s="80">
         <v>0.63</v>
       </c>
-      <c r="J16" s="80"/>
+      <c r="J16" s="80">
+        <v>0.61</v>
+      </c>
       <c r="K16" s="80"/>
       <c r="L16" s="80"/>
       <c r="M16" s="80"/>
       <c r="N16" s="79">
         <f>AVERAGE(B16:M16)</f>
-        <v>0.62875000000000003</v>
+        <v>0.62666666666666671</v>
       </c>
       <c r="O16" s="79">
         <f>1-N16</f>
-        <v>0.37124999999999997</v>
+        <v>0.37333333333333329</v>
       </c>
       <c r="P16" s="69"/>
       <c r="Q16" s="16"/>
@@ -34957,17 +34975,19 @@
       <c r="I17" s="80">
         <v>0.8</v>
       </c>
-      <c r="J17" s="80"/>
+      <c r="J17" s="80">
+        <v>0.81</v>
+      </c>
       <c r="K17" s="80"/>
       <c r="L17" s="80"/>
       <c r="M17" s="80"/>
       <c r="N17" s="79">
         <f>AVERAGE(B17:M17)</f>
-        <v>0.81687499999999991</v>
+        <v>0.81611111111111101</v>
       </c>
       <c r="O17" s="79">
         <f>1-N17</f>
-        <v>0.18312500000000009</v>
+        <v>0.18388888888888899</v>
       </c>
       <c r="P17" s="70"/>
       <c r="Q17" s="18"/>
@@ -35145,14 +35165,14 @@
       </c>
       <c r="B51" s="22">
         <f>J16</f>
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="C51" s="22">
         <v>0.63</v>
       </c>
       <c r="D51" s="22">
         <f>J17</f>
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="E51" s="24">
         <v>0.77</v>
@@ -35221,14 +35241,14 @@
       </c>
       <c r="B55" s="26">
         <f>N16</f>
-        <v>0.62875000000000003</v>
+        <v>0.62666666666666671</v>
       </c>
       <c r="C55" s="26">
         <v>0.64416666666666667</v>
       </c>
       <c r="D55" s="26">
         <f>N17</f>
-        <v>0.81687499999999991</v>
+        <v>0.81611111111111101</v>
       </c>
       <c r="E55" s="27">
         <v>0.85583333333333345</v>
@@ -35263,11 +35283,11 @@
       </c>
       <c r="B1" s="62">
         <f>Total!J7</f>
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="C1" s="32">
         <f>D1-B1</f>
-        <v>1</v>
+        <v>0.32999999999999996</v>
       </c>
       <c r="D1" s="33">
         <v>1</v>
@@ -35279,11 +35299,11 @@
       </c>
       <c r="B2" s="20">
         <f>Total!J8</f>
-        <v>0</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="C2" s="21">
         <f t="shared" ref="C2:C10" si="0">D2-B2</f>
-        <v>1</v>
+        <v>0.43999999999999995</v>
       </c>
       <c r="D2" s="35">
         <v>1</v>
@@ -35295,11 +35315,11 @@
       </c>
       <c r="B3" s="20">
         <f>Total!J9</f>
-        <v>0</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="C3" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.43999999999999995</v>
       </c>
       <c r="D3" s="35">
         <v>1</v>
@@ -35311,11 +35331,11 @@
       </c>
       <c r="B4" s="20">
         <f>Total!J10</f>
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C4" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="D4" s="35">
         <v>1</v>
@@ -35327,11 +35347,11 @@
       </c>
       <c r="B5" s="20">
         <f>Total!J11</f>
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="C5" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.35</v>
       </c>
       <c r="D5" s="35">
         <v>1</v>
@@ -35343,11 +35363,11 @@
       </c>
       <c r="B6" s="20">
         <f>Total!J12</f>
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="C6" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.35</v>
       </c>
       <c r="D6" s="35">
         <v>1</v>
@@ -35359,11 +35379,11 @@
       </c>
       <c r="B7" s="66">
         <f>Total!J14</f>
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="C7" s="37">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D7" s="38">
         <v>1</v>
@@ -35381,11 +35401,11 @@
       </c>
       <c r="B9" s="19">
         <f>Total!B51</f>
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="C9" s="52">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.39</v>
       </c>
       <c r="D9" s="53">
         <v>1</v>
@@ -35397,11 +35417,11 @@
       </c>
       <c r="B10" s="51">
         <f>Total!D51</f>
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="C10" s="52">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.18999999999999995</v>
       </c>
       <c r="D10" s="53">
         <v>1</v>
@@ -37268,17 +37288,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="478e6b58-aec7-4dc3-9f41-cb49fd51aa76" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de218069-9b18-4834-8a42-87538bc414b8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001898DE31E6781040974FAF2B6226B070" ma:contentTypeVersion="17" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="8210ab889ee5475f8279815924805e7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="de218069-9b18-4834-8a42-87538bc414b8" xmlns:ns3="346015c6-8778-4c47-bc51-98fcc3d8f0cc" xmlns:ns4="478e6b58-aec7-4dc3-9f41-cb49fd51aa76" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2ca27dc987c1ae5dda2f1ddae95e9c5a" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="de218069-9b18-4834-8a42-87538bc414b8"/>
@@ -37532,6 +37541,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="478e6b58-aec7-4dc3-9f41-cb49fd51aa76" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de218069-9b18-4834-8a42-87538bc414b8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -37542,18 +37562,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E51255DE-438C-4222-9FEF-BAA467D81EC9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1be84928-a867-465e-b2ee-3fc273237fa1"/>
-    <ds:schemaRef ds:uri="478e6b58-aec7-4dc3-9f41-cb49fd51aa76"/>
-    <ds:schemaRef ds:uri="de218069-9b18-4834-8a42-87538bc414b8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4888F49C-1AE0-4EBF-A654-04D8E1B2E686}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37573,6 +37581,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E51255DE-438C-4222-9FEF-BAA467D81EC9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1be84928-a867-465e-b2ee-3fc273237fa1"/>
+    <ds:schemaRef ds:uri="478e6b58-aec7-4dc3-9f41-cb49fd51aa76"/>
+    <ds:schemaRef ds:uri="de218069-9b18-4834-8a42-87538bc414b8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A779E7D-8AEB-4C16-B749-C7560665EC9A}">
   <ds:schemaRefs>

</xml_diff>